<commit_message>
Add base model Objective The model objective function now includes the variable cost, fixed costs, and investment costs. I have also begun adding constraints. The two constraints that are included so far are limits on the maximum retirement and producer availability.
I have restructured the code so that the coefficients of the base model are calculated using functions in a new file "coefficients.jl". This cleans up setup_base file and makes it more readable.
</commit_message>
<xml_diff>
--- a/H2CS2/inputs/input_2region.xlsx
+++ b/H2CS2/inputs/input_2region.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22a94a39b5425449/Documents/02_School/04_ETH/02_Spring_2023_Semester/06_Case_Study/02_Model/Case-Study-ETH/H2CS2/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="6_{3A0D81B4-BF84-4820-B023-16D5A585C192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31024F2B-82E1-4254-BB13-808603946D4D}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="6_{3A0D81B4-BF84-4820-B023-16D5A585C192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E922D88F-CA2E-4833-9782-63D4397EFE84}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="6" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
+    <workbookView minimized="1" xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8904" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
   </bookViews>
   <sheets>
     <sheet name="universal" sheetId="6" r:id="rId1"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052EB23E-145E-400C-A0E4-F392175696F5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -715,7 +715,7 @@
         <v>0.06</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1822,27 +1822,27 @@
       </c>
       <c r="D3">
         <f ca="1">0.85+0.05*RAND()</f>
-        <v>0.86053911044626552</v>
+        <v>0.88702517329743691</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:I3" ca="1" si="0">0.85+0.05*RAND()</f>
-        <v>0.88080840928592119</v>
+        <v>0.89693961414510959</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85344075098649574</v>
+        <v>0.86893697589102747</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86524444247385424</v>
+        <v>0.89372779939521296</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85992376391546288</v>
+        <v>0.86094218268138689</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85119110814610499</v>
+        <v>0.87372490573862716</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1858,27 +1858,27 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:I38" ca="1" si="2">0.85+0.05*RAND()</f>
-        <v>0.87085410168995514</v>
+        <v>0.8822608056706972</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89474656364832317</v>
+        <v>0.86485166348438847</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89021623887971002</v>
+        <v>0.85088071257613973</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8911958816628528</v>
+        <v>0.85623764283602799</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88164018166698843</v>
+        <v>0.89124822588378272</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87223052462302042</v>
+        <v>0.89709846494330248</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1894,27 +1894,27 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86607134574444988</v>
+        <v>0.88749695379294191</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87781672877802752</v>
+        <v>0.89617263282810045</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.871638583127751</v>
+        <v>0.89810611819590658</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85007155936844758</v>
+        <v>0.88097498034425004</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89586296822723765</v>
+        <v>0.89719454894444695</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85719124640813327</v>
+        <v>0.8706952198708886</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1930,27 +1930,27 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85769497258876526</v>
+        <v>0.87276527946267202</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89215114195621348</v>
+        <v>0.89688865174513932</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89012256691492375</v>
+        <v>0.85959312829449064</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89822443094875071</v>
+        <v>0.87165895912968405</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87737405019723891</v>
+        <v>0.88004221828673146</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86655376958280728</v>
+        <v>0.86164746443331575</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1966,27 +1966,27 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8636185544047208</v>
+        <v>0.8914129474967154</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85153740081756535</v>
+        <v>0.86351813349288653</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88875578427113155</v>
+        <v>0.87537066698805521</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8622297596100319</v>
+        <v>0.865283436428678</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88390184505161262</v>
+        <v>0.85565086614062802</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86248401378683792</v>
+        <v>0.85912229191643641</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2002,27 +2002,27 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89102826494778853</v>
+        <v>0.8530860693218999</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87480224938319662</v>
+        <v>0.88263026898876729</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89267089021779411</v>
+        <v>0.89438458251154018</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88475411034095386</v>
+        <v>0.857621190575655</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85957268129855757</v>
+        <v>0.89287660793515544</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89934484147089166</v>
+        <v>0.85108092556802406</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2038,27 +2038,27 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87129765358028299</v>
+        <v>0.86124501052498348</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88229128674005153</v>
+        <v>0.8741883814209882</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86872015976333927</v>
+        <v>0.88640577298839518</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87900604544613181</v>
+        <v>0.88737706397706373</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88209575192370837</v>
+        <v>0.88120427482020558</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88447095451116886</v>
+        <v>0.86785034244814907</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2074,27 +2074,27 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86963577610943577</v>
+        <v>0.89099849798964192</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89214904125251382</v>
+        <v>0.88742671546915852</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88591197666808708</v>
+        <v>0.8919427252822083</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89541514536677391</v>
+        <v>0.88884151554851565</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85564030217474307</v>
+        <v>0.89321802998447675</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85899834626639382</v>
+        <v>0.8655770620738763</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2110,27 +2110,27 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85495206546456692</v>
+        <v>0.88404633295526003</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85215223614997482</v>
+        <v>0.87032610198229221</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89506502698475487</v>
+        <v>0.85814351051734905</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87107053548997804</v>
+        <v>0.88281976000988016</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89303367411358092</v>
+        <v>0.88624102984248032</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88783780612579288</v>
+        <v>0.87781860966792469</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2146,27 +2146,27 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88338927929783972</v>
+        <v>0.86117222451364406</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88738737740270146</v>
+        <v>0.87458011682234693</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88804672224325532</v>
+        <v>0.88288457460261793</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89097396898991144</v>
+        <v>0.85121247258185551</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8724557029385418</v>
+        <v>0.88384304931649604</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87443535755613588</v>
+        <v>0.85351301533778856</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2182,27 +2182,27 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88041290295378472</v>
+        <v>0.89929377760936979</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85977356574263775</v>
+        <v>0.86333388127257438</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87090606209304133</v>
+        <v>0.89649252163529425</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85665871201141297</v>
+        <v>0.85626402092322074</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86924317582383759</v>
+        <v>0.89022486850748095</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85038509274458218</v>
+        <v>0.85616201896791222</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2218,27 +2218,27 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87510107659242664</v>
+        <v>0.89225002663580166</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88399078681258969</v>
+        <v>0.89154286814905037</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86001141632687061</v>
+        <v>0.88404831504786396</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85048662655237739</v>
+        <v>0.86458676573027171</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85450436456910595</v>
+        <v>0.87965036888254022</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86382666572272226</v>
+        <v>0.86588875603202431</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2254,27 +2254,27 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88869880142555102</v>
+        <v>0.85623669951823178</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89440755672421579</v>
+        <v>0.8766534058428842</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87370715763403273</v>
+        <v>0.8608791809290478</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8516207086297708</v>
+        <v>0.851425058284911</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89622359257496709</v>
+        <v>0.85462733596106655</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88688795893483863</v>
+        <v>0.89136729312035534</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2290,27 +2290,27 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87322615204671938</v>
+        <v>0.86885116435592424</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8779499671187353</v>
+        <v>0.87500289352506944</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8902893771817062</v>
+        <v>0.87867239865446922</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88948716279186546</v>
+        <v>0.8864372986192246</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85647095306271159</v>
+        <v>0.88198029725219795</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86539376563679016</v>
+        <v>0.89458863367319341</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2326,27 +2326,27 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8964950287762925</v>
+        <v>0.8709726799978309</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85890237059072561</v>
+        <v>0.87065973489095061</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86022194128342022</v>
+        <v>0.89520530792663322</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88093213223871758</v>
+        <v>0.86275459677859301</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89412483965508716</v>
+        <v>0.89054082350630093</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88967162732096439</v>
+        <v>0.86430133359285288</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2362,27 +2362,27 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85808520733484595</v>
+        <v>0.89933614055616218</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87809472251229637</v>
+        <v>0.88455213422619461</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86556830183155764</v>
+        <v>0.86796804241010361</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86645807457557589</v>
+        <v>0.85938663690426675</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89338545779976852</v>
+        <v>0.85810064934570152</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87487056015632536</v>
+        <v>0.87894034508966079</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2398,27 +2398,27 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86958294707180461</v>
+        <v>0.85061571931297597</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89443502312982059</v>
+        <v>0.86669948789756279</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8525198032925897</v>
+        <v>0.85948705046993656</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89263996280258262</v>
+        <v>0.86294060534046191</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88537890520929929</v>
+        <v>0.87882631152295121</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85600004088487891</v>
+        <v>0.86196681461596536</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2434,27 +2434,27 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87999487237631258</v>
+        <v>0.89935622296017803</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86469541811676254</v>
+        <v>0.87674650342675453</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8638511943701328</v>
+        <v>0.89646627235554388</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89892241592825184</v>
+        <v>0.89924902913276372</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86601098853969194</v>
+        <v>0.86789003576070878</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85083197266030042</v>
+        <v>0.8993701356096484</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2470,27 +2470,27 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86539816315966234</v>
+        <v>0.87502664144964204</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="2"/>
-        <v>0.896976911721449</v>
+        <v>0.88336784231810439</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89412589993064862</v>
+        <v>0.85345243460549192</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86209425370774229</v>
+        <v>0.87231823478168402</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85120669994625253</v>
+        <v>0.88618114449881014</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89684893219126582</v>
+        <v>0.85422923304911114</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2506,27 +2506,27 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88893711360078365</v>
+        <v>0.88758756573185904</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86046731525547226</v>
+        <v>0.89241172282770675</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88468482031486551</v>
+        <v>0.86639214057874137</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87496123044055341</v>
+        <v>0.88983844803566248</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86669256916636039</v>
+        <v>0.88653189098957419</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89381555761457898</v>
+        <v>0.8741812077428891</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2542,27 +2542,27 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88307940867741952</v>
+        <v>0.89443191997730176</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8661096833294033</v>
+        <v>0.89407006209719042</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86220780412602027</v>
+        <v>0.87919609466609672</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86961969230408454</v>
+        <v>0.88333645522974458</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89981524877196672</v>
+        <v>0.85331027560964612</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87772020582419252</v>
+        <v>0.862548978588073</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2578,27 +2578,27 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87694107581328551</v>
+        <v>0.88097713546774936</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87863849868074606</v>
+        <v>0.86245052905142672</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8636603496230173</v>
+        <v>0.88649392028392238</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85217759028309992</v>
+        <v>0.87355534385928468</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89022034235356517</v>
+        <v>0.87454345670571509</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86842269362199132</v>
+        <v>0.87177155400159312</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2614,27 +2614,27 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88151636610853923</v>
+        <v>0.88270662541121114</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88489405513530017</v>
+        <v>0.85880932414359523</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87619874776397666</v>
+        <v>0.88171594016820365</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87260603226594013</v>
+        <v>0.86186425051028437</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87205508509906782</v>
+        <v>0.87645001077930473</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85128741818415332</v>
+        <v>0.86618344214273935</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2650,27 +2650,27 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88716303049904877</v>
+        <v>0.85029347147267431</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88852541043669953</v>
+        <v>0.85445669754240339</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87123676719147369</v>
+        <v>0.8930851723726454</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88992124222236946</v>
+        <v>0.86824056260231885</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88847735896084867</v>
+        <v>0.8669484887265152</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85087177139319881</v>
+        <v>0.87615187422217944</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2686,27 +2686,27 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.877297617134568</v>
+        <v>0.86226539250379086</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85830645788569282</v>
+        <v>0.86151690700536121</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8825060343064659</v>
+        <v>0.8813267249635377</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87931763271139451</v>
+        <v>0.89819324179463822</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86051154221113479</v>
+        <v>0.8917621732589659</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8997187099141255</v>
+        <v>0.86057536191886286</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2722,27 +2722,27 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89112089301806297</v>
+        <v>0.89421468013839789</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88514240887046769</v>
+        <v>0.88398352029113392</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89153859469905838</v>
+        <v>0.88176597639544563</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86450480776875105</v>
+        <v>0.85622614103440342</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.887902271541821</v>
+        <v>0.87108562080097096</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8891592858820111</v>
+        <v>0.87467486965459595</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2758,27 +2758,27 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85298355695424022</v>
+        <v>0.86211565567812254</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86550969846915338</v>
+        <v>0.89940907027622596</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8511305850712535</v>
+        <v>0.85752269501842637</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85346795906011219</v>
+        <v>0.85081403005836509</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86519692497176603</v>
+        <v>0.86404845890771764</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85832093245989594</v>
+        <v>0.87038815649737411</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2794,27 +2794,27 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88551744943271526</v>
+        <v>0.85684224382241414</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87707942933957517</v>
+        <v>0.89869419682437479</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87169851199615411</v>
+        <v>0.86570211721662005</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89940748049106856</v>
+        <v>0.87589544539346942</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87584938814806956</v>
+        <v>0.89896337317098396</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8769509068443393</v>
+        <v>0.88007131612984291</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2830,27 +2830,27 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8897413591821669</v>
+        <v>0.86516896362144013</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86265867750332093</v>
+        <v>0.87549204628429966</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86227247563945975</v>
+        <v>0.89666268835725804</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87067415337848697</v>
+        <v>0.86241904916803758</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88424734048443121</v>
+        <v>0.86166881707471865</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89591340453333246</v>
+        <v>0.88674949275716741</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2866,27 +2866,27 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87721602103511276</v>
+        <v>0.88426783773857898</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87207834800186979</v>
+        <v>0.88848975540327013</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88799917209410584</v>
+        <v>0.88782542271900533</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86985297541089901</v>
+        <v>0.89923127115663148</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87621444120273639</v>
+        <v>0.89216025582768865</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86020504857657321</v>
+        <v>0.85621667479056429</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2902,27 +2902,27 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89574147869192289</v>
+        <v>0.88141702009443623</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87657880166414659</v>
+        <v>0.88488539598916582</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88601289413407591</v>
+        <v>0.88604791668266847</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85922872482456147</v>
+        <v>0.88768774675234075</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88348363503013516</v>
+        <v>0.87460961748347321</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89324125282597933</v>
+        <v>0.85263451034315196</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2938,27 +2938,27 @@
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88155952693127915</v>
+        <v>0.87345746338061603</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89462430617753741</v>
+        <v>0.8714623701731975</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8794572593356248</v>
+        <v>0.88755613263460431</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89736078028566812</v>
+        <v>0.8663184581646064</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89719570700979034</v>
+        <v>0.884762644975298</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89555541688073748</v>
+        <v>0.8746193651285844</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2974,27 +2974,27 @@
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="2"/>
-        <v>0.898409780425101</v>
+        <v>0.88475860572026654</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86106323899685011</v>
+        <v>0.8841671191123589</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88566717067049805</v>
+        <v>0.86548128281041881</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87931256549313852</v>
+        <v>0.87625003922753575</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89162259845026315</v>
+        <v>0.87461427221004528</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89473704137756049</v>
+        <v>0.8947994274084079</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3010,27 +3010,27 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85732031948920018</v>
+        <v>0.86153913298200524</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88024137145078307</v>
+        <v>0.89623904706892565</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85524971198395416</v>
+        <v>0.88278998714994805</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="2"/>
-        <v>0.870986971331426</v>
+        <v>0.89100848565717439</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86943274075539856</v>
+        <v>0.86503341269984668</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86395191125319803</v>
+        <v>0.87366592636680751</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3046,27 +3046,27 @@
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86879969262393164</v>
+        <v>0.88573842204387199</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88810444418225876</v>
+        <v>0.88702143980890746</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86033286134831399</v>
+        <v>0.86478556628442926</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89828931216606944</v>
+        <v>0.89812310023505848</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89779492888895118</v>
+        <v>0.8662515221502024</v>
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86864341893277608</v>
+        <v>0.88194568555638897</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3082,27 +3082,27 @@
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87578096446684373</v>
+        <v>0.85951338441027481</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87556840644179101</v>
+        <v>0.86894665460628229</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86279075242362069</v>
+        <v>0.87480814780531402</v>
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88239184578305219</v>
+        <v>0.87670949027022183</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8686155825708276</v>
+        <v>0.88703072863745414</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85927463425947503</v>
+        <v>0.89748377712839322</v>
       </c>
     </row>
   </sheetData>
@@ -3114,7 +3114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A855EF-8EC8-4BC2-8D57-3E0F51401541}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3176,19 +3176,19 @@
       </c>
       <c r="C3">
         <f ca="1">10 +5*RAND()</f>
-        <v>14.372406800074298</v>
+        <v>10.743731594117937</v>
       </c>
       <c r="D3">
         <f ca="1">10 +5*RAND()</f>
-        <v>14.785168455925655</v>
+        <v>10.619390464250893</v>
       </c>
       <c r="E3">
         <f ca="1">10 +5*RAND()</f>
-        <v>10.792254108111967</v>
+        <v>11.367804270141203</v>
       </c>
       <c r="F3">
         <f ca="1">10 +5*RAND()</f>
-        <v>10.182876582759219</v>
+        <v>13.668527547166043</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3200,19 +3200,19 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:F38" ca="1" si="0">10 +5*RAND()</f>
-        <v>13.24922169753013</v>
+        <v>11.780879302651879</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>14.281413349454928</v>
+        <v>10.800449393391853</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>14.150280061193889</v>
+        <v>14.279064960601936</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.182544359926881</v>
+        <v>13.779087665689014</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3224,19 +3224,19 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>11.292665794068819</v>
+        <v>12.780844640387755</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>14.126364249193966</v>
+        <v>10.677842216670376</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>14.844976163683542</v>
+        <v>10.1069623731833</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>12.222632380783253</v>
+        <v>12.409851905806043</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3248,19 +3248,19 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>11.225682485199899</v>
+        <v>13.258087870706596</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>14.255288058715202</v>
+        <v>10.614756516896927</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>11.785443598477915</v>
+        <v>12.254160243696109</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>12.101592795931492</v>
+        <v>13.415191338158682</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3272,19 +3272,19 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.066644418789867</v>
+        <v>14.460676501915863</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>14.298387335687602</v>
+        <v>10.055930211019122</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.661030426936486</v>
+        <v>14.796757570228724</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.155864669504139</v>
+        <v>14.397007875723752</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3296,19 +3296,19 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>14.017603118893154</v>
+        <v>12.841997644113682</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>10.103939855392747</v>
+        <v>13.352551505460625</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>11.235025613911382</v>
+        <v>10.590787824045611</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>14.31081992665322</v>
+        <v>10.138254984440634</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3320,19 +3320,19 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>11.416055464078932</v>
+        <v>11.352044274143534</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>10.594465646198664</v>
+        <v>10.258223704653274</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>11.55752269798489</v>
+        <v>14.797273428259711</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>10.057988287972343</v>
+        <v>13.739944034642996</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3344,19 +3344,19 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>12.224925322445207</v>
+        <v>11.835265702462483</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>12.82347331076028</v>
+        <v>11.956904478671225</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>14.541457354919267</v>
+        <v>10.812376618015238</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>10.988841458569961</v>
+        <v>10.293217229938854</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3368,19 +3368,19 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>13.897491374193882</v>
+        <v>11.153824071425158</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>10.484759309486492</v>
+        <v>14.037229159882834</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>11.667605600565635</v>
+        <v>11.251142840565432</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>12.067415870474932</v>
+        <v>13.792615128559953</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3392,19 +3392,19 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.555967730319574</v>
+        <v>12.782513080492489</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.465677120430916</v>
+        <v>14.672542447940454</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.183370650092543</v>
+        <v>13.139765221171992</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.473598983957412</v>
+        <v>14.088317275034171</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3416,19 +3416,19 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>11.417349805170108</v>
+        <v>10.353937339229578</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>11.747048011354583</v>
+        <v>11.909061167484735</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>12.33267378714185</v>
+        <v>12.323323012577793</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>11.804736589819843</v>
+        <v>11.619898703186182</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3440,19 +3440,19 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>10.005689206188666</v>
+        <v>14.884355680607229</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>12.749678163304297</v>
+        <v>10.29331259860705</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>10.387714019030799</v>
+        <v>12.196205910545068</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>10.062788818161261</v>
+        <v>12.151760909880201</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3464,19 +3464,19 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>13.092806937948719</v>
+        <v>10.053845765624617</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>14.879392962459653</v>
+        <v>12.774155965839904</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>14.482949388736763</v>
+        <v>12.746641753030811</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>10.260207199070484</v>
+        <v>10.801566612756158</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3488,19 +3488,19 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>14.892398118593782</v>
+        <v>10.332275018394968</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>10.542042783680946</v>
+        <v>12.369359119395325</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>11.762327967864605</v>
+        <v>10.449792701032333</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>12.697859759211633</v>
+        <v>11.416257912901386</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3512,19 +3512,19 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>11.037436493063138</v>
+        <v>10.757569960503684</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>13.689159391312232</v>
+        <v>12.754712800684828</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>10.112795328763214</v>
+        <v>13.846649148954413</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>13.118111906014752</v>
+        <v>10.497868980254207</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3536,19 +3536,19 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>12.324845974894517</v>
+        <v>13.349629688447724</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>14.404666494241097</v>
+        <v>11.421196343743821</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>11.054157605262994</v>
+        <v>13.581552425703663</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>12.405011900441433</v>
+        <v>13.829045247984086</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3560,19 +3560,19 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>11.12428951878076</v>
+        <v>13.136914797315256</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>12.945071273389914</v>
+        <v>13.757527587962018</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>13.642004062285029</v>
+        <v>13.174333205225519</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>13.136910175549824</v>
+        <v>11.665557911188113</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3584,19 +3584,19 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>10.693992274859315</v>
+        <v>10.562860820396329</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>14.718580589805766</v>
+        <v>13.47085442900328</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>13.671164829502807</v>
+        <v>13.728733464529872</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="0"/>
-        <v>11.567905803197519</v>
+        <v>12.222410304546031</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3608,19 +3608,19 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>10.4859842922362</v>
+        <v>10.362640062179933</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>11.119613003733999</v>
+        <v>13.836848072834037</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>10.175213385673095</v>
+        <v>12.26106281794136</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>13.957146913213807</v>
+        <v>10.9395111841255</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3632,19 +3632,19 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>10.872108466210058</v>
+        <v>10.811103586700973</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>13.701758691364489</v>
+        <v>13.029766945910644</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>11.997417553194595</v>
+        <v>10.994024386469805</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>10.572290545095317</v>
+        <v>14.304420591377264</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3656,19 +3656,19 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>11.358452011246429</v>
+        <v>11.676914697124031</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>10.511467303478623</v>
+        <v>12.703098707107433</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>10.860917644747865</v>
+        <v>13.939599786124734</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>13.407560832650326</v>
+        <v>11.199400345839916</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3680,19 +3680,19 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>10.79942411750261</v>
+        <v>13.019273002107346</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>14.68654402865084</v>
+        <v>14.032874040311075</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>14.07188171193965</v>
+        <v>14.049608955281766</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>10.064176147859483</v>
+        <v>13.648556066743932</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3704,19 +3704,19 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>14.802818883098617</v>
+        <v>13.199927614623807</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>14.069315035162145</v>
+        <v>14.240126287795515</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>14.860154651913476</v>
+        <v>10.224862388285805</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>11.393453434101255</v>
+        <v>10.015738588219628</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3728,19 +3728,19 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>14.757132938600382</v>
+        <v>11.900467479936234</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>10.271642983443787</v>
+        <v>13.627645593612517</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>11.00527557573</v>
+        <v>12.413207598357515</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="0"/>
-        <v>11.279554349361376</v>
+        <v>13.302735082806997</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3752,19 +3752,19 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>13.430064815604721</v>
+        <v>14.257666986768152</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>14.717197958774163</v>
+        <v>13.002129418201399</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>10.141061012768278</v>
+        <v>10.309104445624078</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="0"/>
-        <v>14.785608231453896</v>
+        <v>10.311274963677052</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3776,19 +3776,19 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>14.306290609618983</v>
+        <v>13.089348002168268</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>12.85139045894346</v>
+        <v>11.304727198595119</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>12.515735324723385</v>
+        <v>12.727572928686419</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="0"/>
-        <v>11.726905433524522</v>
+        <v>14.385851359644128</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3800,19 +3800,19 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>10.583593712803822</v>
+        <v>13.22641517792192</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>12.844860944871327</v>
+        <v>14.913303375011804</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>11.189882993956878</v>
+        <v>11.379842103263353</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="0"/>
-        <v>10.933001887139053</v>
+        <v>11.373581778155655</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3824,19 +3824,19 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>13.1714472374944</v>
+        <v>14.466784715192286</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>14.351905246999975</v>
+        <v>11.605636336423187</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>14.809530413008279</v>
+        <v>11.25962083054071</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>10.743235058817756</v>
+        <v>14.72788071018633</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3848,19 +3848,19 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>13.66652668287589</v>
+        <v>13.954094737090044</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>12.877577028165414</v>
+        <v>13.245873437362906</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>13.496949632628642</v>
+        <v>12.739735440335712</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="0"/>
-        <v>14.21915951494616</v>
+        <v>14.105448676602734</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3872,19 +3872,19 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>11.870967232747859</v>
+        <v>14.996953693768321</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>12.968919070891832</v>
+        <v>12.635709268420364</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>12.896416019983619</v>
+        <v>13.803541764002485</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="0"/>
-        <v>13.04855885317388</v>
+        <v>11.386504803606401</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3896,19 +3896,19 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>10.338211937813432</v>
+        <v>13.994119387239913</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>11.55708750632761</v>
+        <v>12.474345898752869</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>14.126522913961708</v>
+        <v>14.141821546542761</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="0"/>
-        <v>14.527703342533394</v>
+        <v>11.832432529473344</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3920,19 +3920,19 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>14.73826469838443</v>
+        <v>14.387700246325196</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>11.567376765073904</v>
+        <v>12.966124757940579</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>11.465209801367431</v>
+        <v>14.534989815998982</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="0"/>
-        <v>13.736829827424472</v>
+        <v>13.407589172740904</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3944,19 +3944,19 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>14.451786682235285</v>
+        <v>13.794157317484057</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="0"/>
-        <v>12.859633933415603</v>
+        <v>14.776624391608227</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>11.047404750739702</v>
+        <v>14.488552864687286</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="0"/>
-        <v>13.453753632954275</v>
+        <v>14.262081118038003</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3968,19 +3968,19 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>12.612986935703486</v>
+        <v>12.523577435892202</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>11.515438980973158</v>
+        <v>10.787728474610551</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="0"/>
-        <v>12.789864786680837</v>
+        <v>13.117105915159605</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="0"/>
-        <v>10.892627786355607</v>
+        <v>10.337285479096391</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3992,19 +3992,19 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="0"/>
-        <v>12.091168710946292</v>
+        <v>13.470369475952367</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>11.821022904876468</v>
+        <v>14.596347203281738</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="0"/>
-        <v>14.191012103751312</v>
+        <v>14.799640111451458</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="0"/>
-        <v>11.577757621264414</v>
+        <v>10.733470608342667</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -4016,19 +4016,19 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="0"/>
-        <v>11.847585645961718</v>
+        <v>13.510637673071061</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
-        <v>13.147513906114817</v>
+        <v>10.659549003516251</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="0"/>
-        <v>10.596758736084993</v>
+        <v>12.741648881228729</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="0"/>
-        <v>14.603490885352866</v>
+        <v>14.434185519671896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>